<commit_message>
new feature generate qrcode base64 image for short link
</commit_message>
<xml_diff>
--- a/datasource/data.xlsx
+++ b/datasource/data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="172">
   <si>
     <t>Timestamp</t>
   </si>
@@ -425,6 +425,108 @@
   </si>
   <si>
     <t>https://drive.google.com/open?id=1UKjyZH4cQlI3egG1Wd5TJiENF6mKFrTd</t>
+  </si>
+  <si>
+    <t>rahmatsuar@gmail.com</t>
+  </si>
+  <si>
+    <t>Seni Budaya</t>
+  </si>
+  <si>
+    <t>Rahmansyah, S.Pd</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/forms/d/e/1FAIpQLSe0oUpxSCrlasfTAbuzYvd9JY6pZp99ym4MxY_M8Jnd7c2DOw/viewform?usp=dialog</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1oTdirStvt9p2_YW1MwyyDIln679ZwjrA</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1DgY1V2HNU4ssTIaKfYovuf_WuEdDwflD</t>
+  </si>
+  <si>
+    <t>muhikram97@guru.smk.belajar.id</t>
+  </si>
+  <si>
+    <t>Pendidikan Agama Islam</t>
+  </si>
+  <si>
+    <t>Muh. Hayan Aliyul Ikram, S.Pd</t>
+  </si>
+  <si>
+    <t>https://forms.gle/8FafVdiK882mRyMQ9</t>
+  </si>
+  <si>
+    <t>JANGAN TANYA SAYA</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1RMnFtAEiAxcWM_NvnsPUCafPTiLZkLpB</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=16x-BaIuZ3grVptPiqBXcsXcfOO410OoP</t>
+  </si>
+  <si>
+    <t>hasbia082@gmail.com</t>
+  </si>
+  <si>
+    <t>Sejarah</t>
+  </si>
+  <si>
+    <t>Kurniah</t>
+  </si>
+  <si>
+    <t>Kelas XII semua kelas</t>
+  </si>
+  <si>
+    <t>https://forms.gle/bcgCoRxvjXYspZ4r6</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1Iyu3pa1ukQw4CKGInSFhcAkzqBUlDLmF</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1ey-w1GvtdP02mZa3BNmu4HVJPgxU0CdA</t>
+  </si>
+  <si>
+    <t>ardan43@guru.smk.belajar.id</t>
+  </si>
+  <si>
+    <t>INFORMATIKA</t>
+  </si>
+  <si>
+    <t>ARDAN, S.KOM</t>
+  </si>
+  <si>
+    <t>XII SEMUA JURUSAN</t>
+  </si>
+  <si>
+    <t>https://forms.gle/szdGBkRcqXWYQjcG9</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1zE1UiltNmbdyti2KGrHvVdJ2Sx_uH3kX</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1T2kBeZzvoxzNXVg5WJy6UQzL7XAIt29e</t>
+  </si>
+  <si>
+    <t>usmana06@guru.smk.belajar.id</t>
+  </si>
+  <si>
+    <t>DASAR TJKT</t>
+  </si>
+  <si>
+    <t>USMAN, A., S.Kom</t>
+  </si>
+  <si>
+    <t>https://s.id/26EwZ</t>
+  </si>
+  <si>
+    <t>t0ken1zm7</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1g1SKbg-3IG8_TrVdzOC958zgSnsR32Ii</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1uTXxHOv2n3PwLi_M9ZABuUmo_h9RM7jH</t>
   </si>
 </sst>
 </file>
@@ -434,7 +536,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="16">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -488,6 +590,11 @@
     </font>
     <font>
       <u/>
+      <color rgb="FF434343"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <u/>
       <color rgb="FF0000FF"/>
       <name val="Roboto"/>
     </font>
@@ -495,6 +602,20 @@
       <u/>
       <color rgb="FF0000FF"/>
       <name val="Roboto"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF1155CC"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -679,7 +800,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="31">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -752,8 +873,26 @@
     <xf borderId="11" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="12" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf borderId="11" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="12" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="13" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -813,7 +952,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I19" displayName="Form_Responses1" name="Form_Responses1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I23" displayName="Form_Responses1" name="Form_Responses1" id="1">
   <tableColumns count="9">
     <tableColumn name="Timestamp" id="1"/>
     <tableColumn name="Email Address" id="2"/>
@@ -1041,7 +1180,7 @@
     <col customWidth="1" min="4" max="4" width="22.25"/>
     <col customWidth="1" min="5" max="7" width="18.88"/>
     <col customWidth="1" min="8" max="8" width="19.5"/>
-    <col customWidth="1" min="9" max="15" width="18.88"/>
+    <col customWidth="1" min="9" max="17" width="18.88"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1567,33 +1706,185 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="21">
+      <c r="A19" s="12">
         <v>45719.30979125</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="D19" s="22" t="s">
+      <c r="D19" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="E19" s="22" t="s">
+      <c r="E19" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="F19" s="23" t="s">
+      <c r="F19" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="G19" s="22" t="s">
+      <c r="G19" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="H19" s="23" t="s">
+      <c r="H19" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="I19" s="24" t="s">
+      <c r="I19" s="15" t="s">
         <v>137</v>
       </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="16">
+        <v>45719.560978877314</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="G20" s="17">
+        <v>599270.0</v>
+      </c>
+      <c r="H20" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="I20" s="19" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="12">
+        <v>45720.50556311343</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="H21" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="I21" s="15" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="16">
+        <v>45720.51610724537</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="G22" s="17">
+        <v>172025.0</v>
+      </c>
+      <c r="H22" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="I22" s="19" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="21">
+        <v>45720.53124848379</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="D23" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="E23" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="G23" s="22">
+        <v>1337.0</v>
+      </c>
+      <c r="H23" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="I23" s="25" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="26">
+        <f>NOW()</f>
+        <v>45720.53542</v>
+      </c>
+      <c r="B24" s="27" t="s">
+        <v>165</v>
+      </c>
+      <c r="C24" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="D24" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="E24" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="F24" s="29" t="s">
+        <v>168</v>
+      </c>
+      <c r="G24" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="H24" s="29" t="s">
+        <v>170</v>
+      </c>
+      <c r="I24" s="29" t="s">
+        <v>171</v>
+      </c>
+      <c r="L24" s="27"/>
+      <c r="M24" s="27"/>
+      <c r="N24" s="27"/>
+      <c r="O24" s="27"/>
+      <c r="P24" s="27"/>
+      <c r="Q24" s="27"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1651,10 +1942,26 @@
     <hyperlink r:id="rId52" ref="F19"/>
     <hyperlink r:id="rId53" ref="H19"/>
     <hyperlink r:id="rId54" ref="I19"/>
+    <hyperlink r:id="rId55" ref="F20"/>
+    <hyperlink r:id="rId56" ref="H20"/>
+    <hyperlink r:id="rId57" ref="I20"/>
+    <hyperlink r:id="rId58" ref="F21"/>
+    <hyperlink r:id="rId59" ref="H21"/>
+    <hyperlink r:id="rId60" ref="I21"/>
+    <hyperlink r:id="rId61" ref="F22"/>
+    <hyperlink r:id="rId62" ref="H22"/>
+    <hyperlink r:id="rId63" ref="I22"/>
+    <hyperlink r:id="rId64" ref="F23"/>
+    <hyperlink r:id="rId65" ref="H23"/>
+    <hyperlink r:id="rId66" ref="I23"/>
+    <hyperlink r:id="rId67" ref="F24"/>
+    <hyperlink r:id="rId68" ref="G24"/>
+    <hyperlink r:id="rId69" ref="H24"/>
+    <hyperlink r:id="rId70" ref="I24"/>
   </hyperlinks>
-  <drawing r:id="rId55"/>
+  <drawing r:id="rId71"/>
   <tableParts count="1">
-    <tablePart r:id="rId57"/>
+    <tablePart r:id="rId73"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add html view for links in root url
</commit_message>
<xml_diff>
--- a/datasource/data.xlsx
+++ b/datasource/data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="222">
   <si>
     <t>Timestamp</t>
   </si>
@@ -506,6 +506,156 @@
   </si>
   <si>
     <t>https://drive.google.com/open?id=1T2kBeZzvoxzNXVg5WJy6UQzL7XAIt29e</t>
+  </si>
+  <si>
+    <t>jannamiftahul68@gmail.com</t>
+  </si>
+  <si>
+    <t>PILIHAN</t>
+  </si>
+  <si>
+    <t>MIFTAHUL JANNA</t>
+  </si>
+  <si>
+    <t>Kelas XII tjkt 1 dan XII tjkt 2</t>
+  </si>
+  <si>
+    <t>https://forms.gle/QaJ5G7BihjMhzJFR6</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1HjTX7fox8HKtx_FzW1GjebqJ_OgPiTOP</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1NbXatoSesneP0uxvfHHDFsxXTSGYj23X</t>
+  </si>
+  <si>
+    <t>Mapel Pilihan TJKT</t>
+  </si>
+  <si>
+    <t>Miftahul Janna</t>
+  </si>
+  <si>
+    <t>Kelas XII TJKT 1 &amp; XII TJKT 2</t>
+  </si>
+  <si>
+    <t>https://forms.gle/yGT46VypvcMiWLNM8</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1rLgYGMeUIOV-N-xR-21xPlqGfpsc-l-h</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1rm4mhP7JBwoLKiCl29qzr0NJQZ27MF9R</t>
+  </si>
+  <si>
+    <t>nurhasdiana32@guru.smk.belajar.id</t>
+  </si>
+  <si>
+    <t>MATA PELAJARAN KONSENTRASI KEAHLIAN (AKL)</t>
+  </si>
+  <si>
+    <t>NURHASDIANA.SE</t>
+  </si>
+  <si>
+    <t>XII AKL</t>
+  </si>
+  <si>
+    <t>https://forms.gle/k3kYY5BQzkPAU14T9</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1bYhI2ibj39--2uu1ozNHosMjZ6sKoNGW</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=10FdABBpR0VRpofnATXIzQZIOkCCRRxEP</t>
+  </si>
+  <si>
+    <t>Dasar-Dasar AKL</t>
+  </si>
+  <si>
+    <t>Yusri Tauwal.SE</t>
+  </si>
+  <si>
+    <t>https://forms.gle/2iunoXRTKHntJ4x38</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1bKuCYvg6y6gYpmACZuciIXAe50Q37eT8</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1ai0Kt4_9m3CxfJDUTKoDsJMmTg7V_lsN</t>
+  </si>
+  <si>
+    <t>Mata Pelajaran Pilihan AKL</t>
+  </si>
+  <si>
+    <t>Arman Suardi. S.Pd</t>
+  </si>
+  <si>
+    <t>https://forms.gle/3xorNr5jHxJR1UhQ6</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=17nDl7_m1oJBXYDUlbo84A-JBmQky_RCd</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=104hiLxzxO3FsSVcnsiC0ww_FuGMkBgEe</t>
+  </si>
+  <si>
+    <t>sumiati20@guru.smk.belajar.id</t>
+  </si>
+  <si>
+    <t>Projeck kreatif dan kewirausahaan</t>
+  </si>
+  <si>
+    <t>Sumiati.S.Pd</t>
+  </si>
+  <si>
+    <t>XII MPLB</t>
+  </si>
+  <si>
+    <t>https://forms.gle/Gpa5NLpdt9nUK23YA</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1RPWWeeubOxg389xxgXMLos9dd5nnsYSq</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1bNhQ_ZLTqNZRtgdZYUhcVrMv3wgl-cWw</t>
+  </si>
+  <si>
+    <t>Projek Kreatif dan Kewirausahaan</t>
+  </si>
+  <si>
+    <t>XII TO1 dan XII TO 2</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/forms/d/e/1FAIpQLSdqJxc20-8AWlHyP4i84nu0qBG0QhV_5JGpq2ZrB8LBbueijw/viewform?usp=sharing</t>
+  </si>
+  <si>
+    <t>Terbentur Tertumbuk Terbentuk Kunfayakun Akkanreko Baca</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1yrOu1kr3fy8U5f0kk3CBAUU1nDIDFeUP</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1hTgU6wbksR0GbQChGm6t5-iyWb98kPo7</t>
+  </si>
+  <si>
+    <t>nasrah90@guru.smk.belajar.id</t>
+  </si>
+  <si>
+    <t>DASAR-DASAR PROGRAM KEAHLIAN BUSANA</t>
+  </si>
+  <si>
+    <t>Nasrah, S.Pd., Gr</t>
+  </si>
+  <si>
+    <t>Kelas XII BUSANA 1 DAN 2</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/forms/d/e/1FAIpQLSczuVtJRnq-9-V3B1vUqqJEVv3FwhbOf91Qhk47zYA0u9S4Jg/viewform?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1Kf1I0d67v5xKI9_yR87A9iRN0cug7zG4</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1kbGpSal80ClpYTJFAyrKtfE4FVXH9f3A</t>
   </si>
   <si>
     <t>usmana06@guru.smk.belajar.id</t>
@@ -536,7 +686,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -609,12 +759,17 @@
     </font>
     <font>
       <u/>
-      <color rgb="FF1155CC"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF1155CC"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -800,7 +955,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -864,15 +1019,15 @@
     <xf quotePrefix="1" borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="8" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="10" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="11" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
     <xf borderId="11" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
@@ -889,9 +1044,12 @@
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -952,7 +1110,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I23" displayName="Form_Responses1" name="Form_Responses1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I31" displayName="Form_Responses1" name="Form_Responses1" id="1">
   <tableColumns count="9">
     <tableColumn name="Timestamp" id="1"/>
     <tableColumn name="Email Address" id="2"/>
@@ -1178,7 +1336,9 @@
     <col customWidth="1" min="1" max="2" width="18.88"/>
     <col customWidth="1" min="3" max="3" width="19.25"/>
     <col customWidth="1" min="4" max="4" width="22.25"/>
-    <col customWidth="1" min="5" max="7" width="18.88"/>
+    <col customWidth="1" min="5" max="5" width="18.88"/>
+    <col customWidth="1" min="6" max="6" width="28.13"/>
+    <col customWidth="1" min="7" max="7" width="18.88"/>
     <col customWidth="1" min="8" max="8" width="19.5"/>
     <col customWidth="1" min="9" max="17" width="18.88"/>
   </cols>
@@ -1822,69 +1982,301 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="21">
+      <c r="A23" s="12">
         <v>45720.53124848379</v>
       </c>
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="C23" s="22" t="s">
+      <c r="C23" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="D23" s="22" t="s">
+      <c r="D23" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="E23" s="22" t="s">
+      <c r="E23" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="F23" s="23" t="s">
+      <c r="F23" s="21" t="s">
         <v>162</v>
       </c>
-      <c r="G23" s="22">
+      <c r="G23" s="13">
         <v>1337.0</v>
       </c>
-      <c r="H23" s="24" t="s">
+      <c r="H23" s="14" t="s">
         <v>163</v>
       </c>
-      <c r="I23" s="25" t="s">
+      <c r="I23" s="15" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="26">
+      <c r="A24" s="16">
+        <v>45721.521743680554</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="G24" s="17">
+        <v>211121.0</v>
+      </c>
+      <c r="H24" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="I24" s="19" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="12">
+        <v>45721.53458743056</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="G25" s="13">
+        <v>211121.0</v>
+      </c>
+      <c r="H25" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="I25" s="15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="16">
+        <v>45721.61758453704</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="G26" s="17">
+        <v>111222.0</v>
+      </c>
+      <c r="H26" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="I26" s="19" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="12">
+        <v>45721.62255950231</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="G27" s="13">
+        <v>123456.0</v>
+      </c>
+      <c r="H27" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="I27" s="15" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="16">
+        <v>45721.62769337963</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="F28" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="G28" s="17">
+        <v>123321.0</v>
+      </c>
+      <c r="H28" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="I28" s="19" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="12">
+        <v>45722.40375938657</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="G29" s="13">
+        <v>123123.0</v>
+      </c>
+      <c r="H29" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="I29" s="15" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="16">
+        <v>45724.4504808912</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="F30" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="G30" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="H30" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="I30" s="19" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="22">
+        <v>45724.55108892361</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>208</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>209</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="E31" s="23" t="s">
+        <v>211</v>
+      </c>
+      <c r="F31" s="24" t="s">
+        <v>212</v>
+      </c>
+      <c r="G31" s="23">
+        <v>252525.0</v>
+      </c>
+      <c r="H31" s="24" t="s">
+        <v>213</v>
+      </c>
+      <c r="I31" s="25" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="26">
         <f>NOW()</f>
-        <v>45720.53542</v>
-      </c>
-      <c r="B24" s="27" t="s">
-        <v>165</v>
-      </c>
-      <c r="C24" s="27" t="s">
-        <v>166</v>
-      </c>
-      <c r="D24" s="27" t="s">
-        <v>167</v>
-      </c>
-      <c r="E24" s="28" t="s">
+        <v>45725.35324</v>
+      </c>
+      <c r="B32" s="27" t="s">
+        <v>215</v>
+      </c>
+      <c r="C32" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="D32" s="27" t="s">
+        <v>217</v>
+      </c>
+      <c r="E32" s="28" t="s">
         <v>161</v>
       </c>
-      <c r="F24" s="29" t="s">
-        <v>168</v>
-      </c>
-      <c r="G24" s="30" t="s">
-        <v>169</v>
-      </c>
-      <c r="H24" s="29" t="s">
-        <v>170</v>
-      </c>
-      <c r="I24" s="29" t="s">
-        <v>171</v>
-      </c>
-      <c r="L24" s="27"/>
-      <c r="M24" s="27"/>
-      <c r="N24" s="27"/>
-      <c r="O24" s="27"/>
-      <c r="P24" s="27"/>
-      <c r="Q24" s="27"/>
+      <c r="F32" s="29" t="s">
+        <v>218</v>
+      </c>
+      <c r="G32" s="30" t="s">
+        <v>219</v>
+      </c>
+      <c r="H32" s="31" t="s">
+        <v>220</v>
+      </c>
+      <c r="I32" s="31" t="s">
+        <v>221</v>
+      </c>
+      <c r="L32" s="27"/>
+      <c r="M32" s="27"/>
+      <c r="N32" s="27"/>
+      <c r="O32" s="27"/>
+      <c r="P32" s="27"/>
+      <c r="Q32" s="27"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1955,13 +2347,38 @@
     <hyperlink r:id="rId65" ref="H23"/>
     <hyperlink r:id="rId66" ref="I23"/>
     <hyperlink r:id="rId67" ref="F24"/>
-    <hyperlink r:id="rId68" ref="G24"/>
-    <hyperlink r:id="rId69" ref="H24"/>
-    <hyperlink r:id="rId70" ref="I24"/>
+    <hyperlink r:id="rId68" ref="H24"/>
+    <hyperlink r:id="rId69" ref="I24"/>
+    <hyperlink r:id="rId70" ref="F25"/>
+    <hyperlink r:id="rId71" ref="H25"/>
+    <hyperlink r:id="rId72" ref="I25"/>
+    <hyperlink r:id="rId73" ref="D26"/>
+    <hyperlink r:id="rId74" ref="F26"/>
+    <hyperlink r:id="rId75" ref="H26"/>
+    <hyperlink r:id="rId76" ref="I26"/>
+    <hyperlink r:id="rId77" ref="F27"/>
+    <hyperlink r:id="rId78" ref="H27"/>
+    <hyperlink r:id="rId79" ref="I27"/>
+    <hyperlink r:id="rId80" ref="F28"/>
+    <hyperlink r:id="rId81" ref="H28"/>
+    <hyperlink r:id="rId82" ref="I28"/>
+    <hyperlink r:id="rId83" ref="F29"/>
+    <hyperlink r:id="rId84" ref="H29"/>
+    <hyperlink r:id="rId85" ref="I29"/>
+    <hyperlink r:id="rId86" ref="F30"/>
+    <hyperlink r:id="rId87" ref="H30"/>
+    <hyperlink r:id="rId88" ref="I30"/>
+    <hyperlink r:id="rId89" ref="F31"/>
+    <hyperlink r:id="rId90" ref="H31"/>
+    <hyperlink r:id="rId91" ref="I31"/>
+    <hyperlink r:id="rId92" ref="F32"/>
+    <hyperlink r:id="rId93" ref="G32"/>
+    <hyperlink r:id="rId94" ref="H32"/>
+    <hyperlink r:id="rId95" ref="I32"/>
   </hyperlinks>
-  <drawing r:id="rId71"/>
+  <drawing r:id="rId96"/>
   <tableParts count="1">
-    <tablePart r:id="rId73"/>
+    <tablePart r:id="rId98"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>